<commit_message>
analytics corrected and requirements.txt renewed
</commit_message>
<xml_diff>
--- a/grouped_ds.xlsx
+++ b/grouped_ds.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,72 +498,37 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45852</v>
+        <v>45880</v>
       </c>
       <c r="B2" t="n">
         <v>7</v>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>1.97</v>
+        <v>2.75</v>
       </c>
       <c r="I2" t="n">
-        <v>0.28</v>
+        <v>0.39</v>
       </c>
       <c r="J2" t="n">
-        <v>100</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>45859</v>
-      </c>
-      <c r="B3" t="n">
-        <v>35</v>
-      </c>
-      <c r="C3" t="n">
-        <v>32</v>
-      </c>
-      <c r="D3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E3" t="n">
-        <v>30</v>
-      </c>
-      <c r="F3" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>31.4</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="J3" t="n">
-        <v>91.40000000000001</v>
-      </c>
-      <c r="K3" t="n">
-        <v>8.599999999999994</v>
+        <v>28.59999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>